<commit_message>
Mejoras proceso HSA en edición de boleta
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/HSA.xlsx
+++ b/App.Web/App_Data/HSA.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23250" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="25170" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$B$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$P$1</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Id informe</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Id proceso</t>
   </si>
@@ -74,7 +71,7 @@
     <t>N° boleta</t>
   </si>
   <si>
-    <t>Proceso terminado?</t>
+    <t>Estado proceso</t>
   </si>
 </sst>
 </file>
@@ -403,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -411,8 +408,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
@@ -421,61 +418,57 @@
     <col min="11" max="13" width="48.42578125" customWidth="1"/>
     <col min="14" max="14" width="18.28515625" style="3" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:Q1"/>
+  <autoFilter ref="A1:P1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
GD - Mejoras de informes de procesos y hsa
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/HSA.xlsx
+++ b/App.Web/App_Data/HSA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\GestionProcesosV2\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24704F6-814A-490B-AD65-DE545C7583E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25170" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="825" yWindow="-120" windowWidth="23295" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,23 +400,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="48.42578125" customWidth="1"/>
+    <col min="7" max="9" width="28" customWidth="1"/>
     <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="48.42578125" customWidth="1"/>
+    <col min="11" max="13" width="28" customWidth="1"/>
     <col min="14" max="14" width="18.28515625" style="3" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -468,7 +469,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P1"/>
+  <autoFilter ref="A1:P1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>